<commit_message>
Complete report, rename the method
</commit_message>
<xml_diff>
--- a/analiza.xlsx
+++ b/analiza.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\PEA-PrzegladZupelny-ErykMika-264451\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAE7F6A-D858-43EB-93FA-CDA86402DC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213B4030-1BEF-45FB-BA51-280E5F24AF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{C59438C6-7367-4BB4-9D7A-79359F993448}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C59438C6-7367-4BB4-9D7A-79359F993448}"/>
   </bookViews>
   <sheets>
     <sheet name="12" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>N=12</t>
   </si>
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +77,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,17 +108,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -276,7 +295,7 @@
             <c:numRef>
               <c:f>summary!$B$2:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.7060000000000022</c:v>
@@ -381,7 +400,7 @@
             <c:numRef>
               <c:f>summary!$C$2:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.7</c:v>
@@ -1336,8 +1355,8 @@
   <autoFilter ref="A1:C8" xr:uid="{4475EC42-18EE-4DD6-8CE4-32656DC9089A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8D76FAF2-8C81-4338-B850-07B4B3FB48CC}" name="N"/>
-    <tableColumn id="2" xr3:uid="{C4557935-1C5D-49B3-A6F8-7113DD505397}" name="średnia"/>
-    <tableColumn id="3" xr3:uid="{632E18F1-8A10-40C5-99E6-9E92CC469FFA}" name="mediana"/>
+    <tableColumn id="2" xr3:uid="{C4557935-1C5D-49B3-A6F8-7113DD505397}" name="średnia" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{632E18F1-8A10-40C5-99E6-9E92CC469FFA}" name="mediana" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1640,524 +1659,1321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98737A25-1979-4AE8-BAAD-86E8E34CEF8B}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>937451.4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <f>ABS(A1-$A$101)</f>
+        <v>2270.9309999998659</v>
+      </c>
+      <c r="C1" s="3">
+        <f>B1/$A$101</f>
+        <v>2.4283345036367151E-3</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>819752</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <f t="shared" ref="B2:B65" si="0">ABS(A2-$A$101)</f>
+        <v>115428.46900000016</v>
+      </c>
+      <c r="C2" s="3">
+        <f t="shared" ref="C2:C65" si="1">B2/$A$101</f>
+        <v>0.12342908435997302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>877896.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>57284.069000000134</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" si="1"/>
+        <v>6.1254560909783207E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>819084.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>116096.06900000013</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1241429572670001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>811615</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>123565.46900000016</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.13213007873456789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>847797</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>87383.469000000157</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="1"/>
+        <v>9.3440220253359615E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1049621.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>114441.03099999984</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12237320473808978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>777337.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>157842.86900000018</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1687833249648418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>938014.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>2834.1309999998193</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="1"/>
+        <v>3.0305712041124961E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>838815.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>96365.069000000134</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.10304435581620355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>966520.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>31339.630999999819</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3511853635600053E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>805952.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>129228.06900000013</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.13818516669641881</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1018312.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>83132.130999999819</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>8.889421213949647E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>947011.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>11830.930999999866</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2650960314270489E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>825291.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>109888.7690000002</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.11750541488265426</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>886944</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>48236.469000000157</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="1"/>
+        <v>5.1579850733602252E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>833778.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>101402.2690000002</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="1"/>
+        <v>0.10843069585107021</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>918717.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>16462.869000000181</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7603948698377038E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1050628.3999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>115447.93099999975</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12344989531640842</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>941567.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>6386.6309999998193</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="1"/>
+        <v>6.8293032325932998E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>872865.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>62315.269000000204</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="1"/>
+        <v>6.6634485070710125E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>808842.1</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>126338.36900000018</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="1"/>
+        <v>0.13509517487581338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>967044.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>31864.130999999819</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="1"/>
+        <v>3.4072707949164636E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>919621.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>15559.069000000134</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6637504220589246E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>919944.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>15235.669000000111</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6291688615237866E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>868999.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>66180.869000000181</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="1"/>
+        <v>7.0768018787612394E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>867973.1</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>67207.369000000181</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="1"/>
+        <v>7.186566788746758E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>882790.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>52389.569000000134</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="1"/>
+        <v>5.6020811743449833E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>882586.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>52593.569000000134</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="1"/>
+        <v>5.6238951457400599E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>815299.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>119880.56900000013</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12818976975448373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>823484.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>111696.16900000011</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="1"/>
+        <v>0.11943808997576498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>898013.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>37167.069000000134</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9743204902197467E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>875061</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>60119.469000000157</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="1"/>
+        <v>6.4286489071234174E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1126334.1000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>191153.63099999994</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="1"/>
+        <v>0.20440293326955689</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1003580.1</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>68399.630999999819</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="1"/>
+        <v>7.3140568336655248E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>937252.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>2071.730999999796</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2153274888376605E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1048705.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>113525.03099999984</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12139371464995792</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1003008.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>67827.630999999819</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="1"/>
+        <v>7.2528921687734491E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1037409.9</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>102229.43099999987</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="1"/>
+        <v>0.10931519037102544</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>897030.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>38149.869000000181</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="1"/>
+        <v>4.0794125053525018E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1012991.2</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>77810.730999999796</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3203973542351414E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1034203.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>99023.130999999819</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1058866542688669</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>933053.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>2126.5690000001341</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2739664380224921E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1097296.3999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>162115.93099999975</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="1"/>
+        <v>0.17335256281961522</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1012342</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>77161.530999999843</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="1"/>
+        <v>8.2509775982072861E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1009250.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>74070.230999999796</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="1"/>
+        <v>7.9204210797092459E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>973862.6</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>38682.130999999819</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="1"/>
+        <v>4.1363279369342573E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1115728.3</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>180547.83099999989</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1930620206312284</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1021897.6</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>86717.130999999819</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="1"/>
+        <v>9.272769681848414E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1026183.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>91003.030999999843</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="1"/>
+        <v>9.731066250486442E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1000033</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>64852.530999999843</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="1"/>
+        <v>6.9347610594720221E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1145856</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>210675.53099999984</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="1"/>
+        <v>0.22527794151355379</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>985286.2</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>50105.730999999796</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="1"/>
+        <v>5.3578675625655936E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>837460.7</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>97719.769000000204</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="1"/>
+        <v>0.10449295322056196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>961249.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>26069.030999999843</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="1"/>
+        <v>2.7875936104478072E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>961173.3</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>25992.830999999889</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="1"/>
+        <v>2.7794454505443576E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>842610.2</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>92570.269000000204</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="1"/>
+        <v>9.8986529411790133E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>881530.7</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>53649.769000000204</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="1"/>
+        <v>5.7368359133257517E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>944084.3</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>8903.8309999998892</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="1"/>
+        <v>9.5209762127740575E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>924603.7</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>10576.769000000204</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1309869432271262E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>954436.7</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>19256.230999999796</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="1"/>
+        <v>2.0590925108381185E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>906713.2</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>28467.269000000204</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="1"/>
+        <v>3.044040155205615E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>906749</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>28431.469000000157</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="1"/>
+        <v>3.0402120170882389E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>951925.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>16744.930999999866</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7905561070907974E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>902348</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>32832.469000000157</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="1"/>
+        <v>3.5108163705673101E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>872157.9</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <f t="shared" ref="B66:B97" si="2">ABS(A66-$A$101)</f>
+        <v>63022.569000000134</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" ref="C66:C97" si="3">B66/$A$101</f>
+        <v>6.7390809676971697E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>963225.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <f t="shared" si="2"/>
+        <v>28045.030999999843</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" si="3"/>
+        <v>2.9988897255295265E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>893449.2</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <f t="shared" si="2"/>
+        <v>41731.269000000204</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="3"/>
+        <v>4.4623760208148872E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>809565.9</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <f t="shared" si="2"/>
+        <v>125614.56900000013</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" si="3"/>
+        <v>0.13432120661621744</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1004781</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <f t="shared" si="2"/>
+        <v>69600.530999999843</v>
+      </c>
+      <c r="C70" s="3">
+        <f t="shared" si="3"/>
+        <v>7.4424705505691899E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>914596.5</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <f t="shared" si="2"/>
+        <v>20583.969000000157</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="shared" si="3"/>
+        <v>2.2010691713879402E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>868378.9</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <f t="shared" si="2"/>
+        <v>66801.569000000134</v>
+      </c>
+      <c r="C72" s="3">
+        <f t="shared" si="3"/>
+        <v>7.1431740946677244E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>891689</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <f t="shared" si="2"/>
+        <v>43491.469000000157</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" si="3"/>
+        <v>4.6505963759600449E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>988760.7</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <f t="shared" si="2"/>
+        <v>53580.230999999796</v>
+      </c>
+      <c r="C74" s="3">
+        <f t="shared" si="3"/>
+        <v>5.7294001292920275E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>875956.6</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <f t="shared" si="2"/>
+        <v>59223.869000000181</v>
+      </c>
+      <c r="C75" s="3">
+        <f t="shared" si="3"/>
+        <v>6.3328812954497424E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>960846.6</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <f t="shared" si="2"/>
+        <v>25666.130999999819</v>
+      </c>
+      <c r="C76" s="3">
+        <f t="shared" si="3"/>
+        <v>2.7445110169425291E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>890633.6</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <f t="shared" si="2"/>
+        <v>44546.869000000181</v>
+      </c>
+      <c r="C77" s="3">
+        <f t="shared" si="3"/>
+        <v>4.7634515985598681E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1116925.3999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <f t="shared" si="2"/>
+        <v>181744.93099999975</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" si="3"/>
+        <v>0.19434209441343639</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>973184.6</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <f t="shared" si="2"/>
+        <v>38004.130999999819</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="3"/>
+        <v>4.0638285614153273E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1012729.6</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <f t="shared" si="2"/>
+        <v>77549.130999999819</v>
+      </c>
+      <c r="C80" s="3">
+        <f t="shared" si="3"/>
+        <v>8.292424143857928E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>819492.8</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <f t="shared" si="2"/>
+        <v>115687.66900000011</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="3"/>
+        <v>0.12370625011416923</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>917183.8</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <f t="shared" si="2"/>
+        <v>17996.669000000111</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="3"/>
+        <v>1.9244059939836178E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>913488.5</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <f t="shared" si="2"/>
+        <v>21691.969000000157</v>
+      </c>
+      <c r="C83" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3195489768082566E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>919881.9</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <f t="shared" si="2"/>
+        <v>15298.569000000134</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6358948360372709E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>926414.7</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <f t="shared" si="2"/>
+        <v>8765.769000000204</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="3"/>
+        <v>9.3733448147966004E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>971714.4</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <f t="shared" si="2"/>
+        <v>36533.930999999866</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="3"/>
+        <v>3.9066182636455234E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>915733.2</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <f t="shared" si="2"/>
+        <v>19447.269000000204</v>
+      </c>
+      <c r="C87" s="3">
+        <f t="shared" si="3"/>
+        <v>2.0795204395997923E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>983636.4</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <f t="shared" si="2"/>
+        <v>48455.930999999866</v>
+      </c>
+      <c r="C88" s="3">
+        <f t="shared" si="3"/>
+        <v>5.1814524154695382E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>910721.8</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <f t="shared" si="2"/>
+        <v>24458.669000000111</v>
+      </c>
+      <c r="C89" s="3">
+        <f t="shared" si="3"/>
+        <v>2.6153956172923567E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>954012.4</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <f t="shared" si="2"/>
+        <v>18831.930999999866</v>
+      </c>
+      <c r="C90" s="3">
+        <f t="shared" si="3"/>
+        <v>2.0137215889610139E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1006568.6</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <f t="shared" si="2"/>
+        <v>71388.130999999819</v>
+      </c>
+      <c r="C91" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6336208214801596E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>845187.7</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <f t="shared" si="2"/>
+        <v>89992.769000000204</v>
+      </c>
+      <c r="C92" s="3">
+        <f t="shared" si="3"/>
+        <v>9.6230376898515171E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>876922.3</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <f t="shared" si="2"/>
+        <v>58258.169000000111</v>
+      </c>
+      <c r="C93" s="3">
+        <f t="shared" si="3"/>
+        <v>6.2296178043898073E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>925742.2</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <f t="shared" si="2"/>
+        <v>9438.269000000204</v>
+      </c>
+      <c r="C94" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0092457352207814E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1002912.6</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <f t="shared" si="2"/>
+        <v>67732.130999999819</v>
+      </c>
+      <c r="C95" s="3">
+        <f t="shared" si="3"/>
+        <v>7.2426802360860479E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1062668.2</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <f t="shared" si="2"/>
+        <v>127487.7309999998</v>
+      </c>
+      <c r="C96" s="3">
+        <f t="shared" si="3"/>
+        <v>0.13632420182633195</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>966809.1</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <f t="shared" si="2"/>
+        <v>31628.630999999819</v>
+      </c>
+      <c r="C97" s="3">
+        <f t="shared" si="3"/>
+        <v>3.38208848970303E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>947823.5</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <f>ABS(A98-$A$101)</f>
+        <v>12643.030999999843</v>
+      </c>
+      <c r="C98" s="3">
+        <f>B98/$A$101</f>
+        <v>1.3519348852012692E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1022475.7</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <f t="shared" ref="B99:B100" si="4">ABS(A99-$A$101)</f>
+        <v>87295.230999999796</v>
+      </c>
+      <c r="C99" s="3">
+        <f t="shared" ref="C99:C100" si="5">B99/$A$101</f>
+        <v>9.3345866272576933E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>880949.9</v>
       </c>
-      <c r="B100" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <f t="shared" si="4"/>
+        <v>54230.569000000134</v>
+      </c>
+      <c r="C100" s="3">
+        <f t="shared" si="5"/>
+        <v>5.7989415730623141E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <f>AVERAGE(A1:A100)</f>
         <v>935180.46900000016</v>
@@ -2165,6 +2981,15 @@
       <c r="B101">
         <f>MEDIAN($A$1:$A$100)</f>
         <v>926078.45</v>
+      </c>
+      <c r="C101" s="4">
+        <f>AVERAGE(C1:C100)</f>
+        <v>6.909198374201711E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5332,8 +6157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD4CA95-F41A-4ACB-9D41-8EE97D9EC387}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5357,11 +6182,11 @@
       <c r="A2">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <f>'6'!A101</f>
         <v>4.7060000000000022</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <f>'6'!B101</f>
         <v>4.7</v>
       </c>
@@ -5370,11 +6195,11 @@
       <c r="A3">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <f>'7'!A101</f>
         <v>26.014999999999997</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <f>'7'!B101</f>
         <v>25.6</v>
       </c>
@@ -5383,11 +6208,11 @@
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f>'8'!A101</f>
         <v>165.49500000000003</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <f>'8'!B101</f>
         <v>164.25</v>
       </c>
@@ -5396,11 +6221,11 @@
       <c r="A5">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <f>'9'!A101</f>
         <v>1270.146</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <f>'9'!B101</f>
         <v>1271.55</v>
       </c>
@@ -5409,11 +6234,11 @@
       <c r="A6">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <f>'10'!A101</f>
         <v>10071.767999999996</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <f>'10'!B101</f>
         <v>9991.0499999999993</v>
       </c>
@@ -5422,11 +6247,11 @@
       <c r="A7">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <f>'11'!A101</f>
         <v>85685.921000000002</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <f>'11'!B101</f>
         <v>84973.85</v>
       </c>
@@ -5435,11 +6260,11 @@
       <c r="A8">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <f>'12'!A101</f>
         <v>935180.46900000016</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <f>'12'!B101</f>
         <v>926078.45</v>
       </c>

</xml_diff>